<commit_message>
18/08/19a datafixtures with csv
</commit_message>
<xml_diff>
--- a/FieldsForEntities.xlsx
+++ b/FieldsForEntities.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>Field Name</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>inputter</t>
+  </si>
+  <si>
+    <t>ManyToOne relation with Inputter class</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D26"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,6 +682,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
180822a with details occurrence
</commit_message>
<xml_diff>
--- a/FieldsForEntities.xlsx
+++ b/FieldsForEntities.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>Field Name</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>ManyToOne relation with Inputter class</t>
+  </si>
+  <si>
+    <t>lastModifiedAt</t>
+  </si>
+  <si>
+    <t>Time of last modification</t>
+  </si>
+  <si>
+    <t>lastModifier</t>
+  </si>
+  <si>
+    <t>ManyToOne relation with Inputter class (condition: Inputter same as creator or Validator)</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,6 +708,34 @@
         <v>47</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
180822b with phylum entity
</commit_message>
<xml_diff>
--- a/FieldsForEntities.xlsx
+++ b/FieldsForEntities.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Field Name</t>
   </si>
@@ -180,6 +180,21 @@
   </si>
   <si>
     <t>ManyToOne relation with Inputter class (condition: Inputter same as creator or Validator)</t>
+  </si>
+  <si>
+    <t>phylum</t>
+  </si>
+  <si>
+    <t>ManyToOne</t>
+  </si>
+  <si>
+    <t>phylumNameWorms</t>
+  </si>
+  <si>
+    <t>Phylum</t>
+  </si>
+  <si>
+    <t>OneToMany</t>
   </si>
 </sst>
 </file>
@@ -497,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,63 +796,102 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B29" t="s">
         <v>45</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>45</v>
       </c>
-      <c r="D25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D30" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>